<commit_message>
Enabling all testcases LogixalQA
</commit_message>
<xml_diff>
--- a/Input_files/Master_executors/LogixalQA/MasterExecutor_Sanity.xlsx
+++ b/Input_files/Master_executors/LogixalQA/MasterExecutor_Sanity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMAN_ReExecuteFailedTcs\KAMAN_ECTEST_IE_SANITY\Input_files\Master_executors\LogixalQA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82DC3806-5CE4-44DA-930E-94FB5B51EB68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9587263-F75C-4B30-8669-57C14DCEF7D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -250,7 +250,7 @@
     <t>RunMode</t>
   </si>
   <si>
-    <t>No</t>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -747,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E9FC807-CD3D-4456-9922-7EB264FD2C96}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>